<commit_message>
uda bisa convert sorek harusnya, tapi nang aku error mysql server has gone away, cobaen neng nggonmu
</commit_message>
<xml_diff>
--- a/doc/sorekschema.xlsx
+++ b/doc/sorekschema.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="sorekschema" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="149">
   <si>
     <t>ColumnName</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>TGL_DJBB</t>
+  </si>
+  <si>
+    <t>System.String (yyyymmdd)</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -2960,7 +2965,7 @@
         <v>255</v>
       </c>
       <c r="F38" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="G38">
         <v>202</v>

</xml_diff>